<commit_message>
Buen trbajo, buscador, planificacion, pruebas y esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Iñigo.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Iñigo.xlsx
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="44">
   <si>
     <t>GP</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>Planificación auditoría</t>
+  </si>
+  <si>
+    <t>Pruebas</t>
   </si>
 </sst>
 </file>
@@ -2361,7 +2364,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2461,11 +2464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="294918568"/>
-        <c:axId val="294918960"/>
+        <c:axId val="300113752"/>
+        <c:axId val="300114144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="294918568"/>
+        <c:axId val="300113752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2506,7 +2509,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294918960"/>
+        <c:crossAx val="300114144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2514,7 +2517,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294918960"/>
+        <c:axId val="300114144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2570,7 +2573,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294918568"/>
+        <c:crossAx val="300113752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3046,6 +3049,102 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10610850" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10610850" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3558,6 +3657,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4038,6 +4233,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4486,6 +4777,102 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5023,6 +5410,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5471,6 +5954,102 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5983,6 +6562,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6431,6 +7106,102 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6943,6 +7714,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7391,6 +8258,102 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7903,6 +8866,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8383,6 +9442,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8651,7 +9806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -20000,7 +21155,7 @@
       </c>
       <c r="G6" s="82">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>17</v>
+        <v>17.25</v>
       </c>
       <c r="H6" s="84">
         <f>Ene!G36</f>
@@ -20016,7 +21171,7 @@
       </c>
       <c r="K6" s="84">
         <f>Abr!G36</f>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="L6" s="84">
         <f>May!G36</f>
@@ -23253,7 +24408,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="B10:F10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23760,7 +24915,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>36</v>
@@ -26129,8 +27284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22:T22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26487,7 +27642,7 @@
         <v>54</v>
       </c>
       <c r="E5" s="119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>40</v>
@@ -26707,7 +27862,7 @@
       </c>
       <c r="G8" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
@@ -26728,7 +27883,7 @@
       <c r="X8" s="20"/>
       <c r="Y8" s="16"/>
       <c r="Z8" s="16">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
@@ -26761,14 +27916,24 @@
     </row>
     <row r="9" spans="1:54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
+      <c r="B9" s="117">
+        <v>85</v>
+      </c>
+      <c r="C9" s="118">
+        <v>2</v>
+      </c>
+      <c r="D9" s="20">
+        <v>56</v>
+      </c>
+      <c r="E9" s="119">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>43</v>
+      </c>
       <c r="G9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -26788,7 +27953,9 @@
       <c r="W9" s="20"/>
       <c r="X9" s="20"/>
       <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
+      <c r="Z9" s="16">
+        <v>0.5</v>
+      </c>
       <c r="AA9" s="20"/>
       <c r="AB9" s="20"/>
       <c r="AC9" s="20"/>
@@ -28363,7 +29530,7 @@
       </c>
       <c r="G36" s="33">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="H36" s="34">
         <f t="shared" ref="H36:AK36" si="1">SUM(H3:H35)</f>
@@ -28439,7 +29606,7 @@
       </c>
       <c r="Z36" s="34">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="AA36" s="51">
         <f t="shared" si="1"/>
@@ -28923,8 +30090,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Creada hoja de esfuerzos de equipo. Arreglado codigo de grupo en la hoja de esfuerzos.
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Iñigo.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Iñigo.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inigo\Desktop\ecatalog\team\efforts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ene" sheetId="1" r:id="rId1"/>
@@ -40,7 +35,7 @@
     <definedName name="Print_Area" localSheetId="9">Oct!$A$1:$AS$37</definedName>
     <definedName name="Print_Area" localSheetId="8">Sep!$A$1:$AR$37</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -50,7 +45,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +68,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +91,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AQ2" authorId="0" shapeId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +114,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +137,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AO2" authorId="0" shapeId="0">
+    <comment ref="AO2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +160,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +183,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AQ2" authorId="0" shapeId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +206,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +229,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AQ2" authorId="0" shapeId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +252,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -280,7 +275,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0" shapeId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -303,7 +298,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AQ2" authorId="0" shapeId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -461,9 +456,6 @@
     <t>Segunda iteración. Destacar modelo</t>
   </si>
   <si>
-    <t>reunion</t>
-  </si>
-  <si>
     <t>Edición de auditoría</t>
   </si>
   <si>
@@ -477,6 +469,9 @@
   </si>
   <si>
     <t>Gestión de proyecto</t>
+  </si>
+  <si>
+    <t>Reunion con el profesor: auditoria externa</t>
   </si>
 </sst>
 </file>
@@ -1853,110 +1848,26 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="36">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFCCFFFF"/>
           <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
         </patternFill>
       </fill>
       <border>
@@ -2347,6 +2258,34 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor indexed="41"/>
           <bgColor indexed="27"/>
         </patternFill>
@@ -2468,7 +2407,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2605,12 +2543,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="319189120"/>
-        <c:axId val="319189512"/>
+        <c:axId val="177764224"/>
+        <c:axId val="177778688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319189120"/>
+        <c:axId val="177764224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,7 +2575,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
@@ -2652,7 +2590,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319189512"/>
+        <c:crossAx val="177778688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2660,7 +2598,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319189512"/>
+        <c:axId val="177778688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,7 +2633,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2717,7 +2654,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319189120"/>
+        <c:crossAx val="177764224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2729,7 +2666,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3338,6 +3274,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10610850" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3994,6 +3978,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4618,6 +4650,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5210,6 +5290,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5891,6 +6019,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6483,6 +6659,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7139,6 +7363,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7731,6 +8003,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8387,6 +8707,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8979,6 +9347,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -9635,6 +10051,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10259,6 +10723,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10305,7 +10817,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10340,7 +10852,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10517,7 +11029,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10588,8 +11100,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -13197,10 +13709,10 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13272,8 +13784,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -16029,12 +16541,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16105,8 +16617,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="154"/>
-      <c r="AR1" s="155"/>
+      <c r="AQ1" s="159"/>
+      <c r="AR1" s="160"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -18814,12 +19326,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18891,8 +19403,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -21648,12 +22160,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22433,12 +22945,12 @@
     <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22452,7 +22964,7 @@
   <dimension ref="A1:AZ43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22508,8 +23020,8 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="154"/>
-      <c r="AP1" s="155"/>
+      <c r="AO1" s="159"/>
+      <c r="AP1" s="160"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
@@ -22853,20 +23365,20 @@
     </row>
     <row r="6" spans="1:52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="156">
+      <c r="B6" s="154">
         <v>84</v>
       </c>
-      <c r="C6" s="157">
+      <c r="C6" s="155">
         <v>2</v>
       </c>
-      <c r="D6" s="157">
+      <c r="D6" s="155">
         <v>41</v>
       </c>
-      <c r="E6" s="159">
-        <v>0</v>
-      </c>
-      <c r="F6" s="158" t="s">
-        <v>49</v>
+      <c r="E6" s="157">
+        <v>0</v>
+      </c>
+      <c r="F6" s="156" t="s">
+        <v>48</v>
       </c>
       <c r="G6" s="11">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:AI6)</f>
@@ -22890,7 +23402,7 @@
       <c r="W6" s="17"/>
       <c r="X6" s="17"/>
       <c r="Y6" s="17"/>
-      <c r="Z6" s="160">
+      <c r="Z6" s="158">
         <v>1</v>
       </c>
       <c r="AA6" s="103"/>
@@ -22922,20 +23434,20 @@
     </row>
     <row r="7" spans="1:52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="156">
+      <c r="B7" s="154">
         <v>84</v>
       </c>
-      <c r="C7" s="157">
+      <c r="C7" s="155">
         <v>2</v>
       </c>
-      <c r="D7" s="157">
+      <c r="D7" s="155">
         <v>41</v>
       </c>
-      <c r="E7" s="159">
-        <v>0</v>
-      </c>
-      <c r="F7" s="158" t="s">
-        <v>50</v>
+      <c r="E7" s="157">
+        <v>0</v>
+      </c>
+      <c r="F7" s="156" t="s">
+        <v>49</v>
       </c>
       <c r="G7" s="11">
         <f t="shared" si="0"/>
@@ -22959,7 +23471,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
-      <c r="Z7" s="160">
+      <c r="Z7" s="158">
         <v>2</v>
       </c>
       <c r="AA7" s="17"/>
@@ -22997,7 +23509,7 @@
       <c r="E8" s="21"/>
       <c r="F8" s="22"/>
       <c r="G8" s="11">
-        <f t="shared" ref="G6:G36" si="1">SUM(H8:AI8)</f>
+        <f t="shared" ref="G8:G36" si="1">SUM(H8:AI8)</f>
         <v>0</v>
       </c>
       <c r="H8" s="16"/>
@@ -25124,30 +25636,30 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G35">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G35">
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5">
-    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25163,7 +25675,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B3" sqref="B3:AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25222,8 +25734,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -28001,30 +28513,30 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G8 G10:G35">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G8 G10:G35">
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3 G9">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3 G9">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28040,7 +28552,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B3" sqref="B3:AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28098,8 +28610,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="154"/>
-      <c r="AR1" s="155"/>
+      <c r="AQ1" s="159"/>
+      <c r="AR1" s="160"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -28884,18 +29396,18 @@
     </row>
     <row r="12" spans="1:54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="156">
+      <c r="B12" s="154">
         <v>84</v>
       </c>
-      <c r="C12" s="157">
+      <c r="C12" s="155">
         <v>2</v>
       </c>
-      <c r="D12" s="157">
+      <c r="D12" s="155">
         <v>44</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="158" t="s">
-        <v>48</v>
+      <c r="F12" s="156" t="s">
+        <v>47</v>
       </c>
       <c r="G12" s="11">
         <f t="shared" si="0"/>
@@ -28915,7 +29427,7 @@
       <c r="S12" s="16"/>
       <c r="T12" s="20"/>
       <c r="U12" s="20"/>
-      <c r="V12" s="157">
+      <c r="V12" s="155">
         <v>2</v>
       </c>
       <c r="W12" s="20"/>
@@ -30869,22 +31381,22 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G11 G13:G35">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G11 G13:G35">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30900,7 +31412,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30959,8 +31471,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -31110,7 +31622,7 @@
     <row r="3" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="116">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="117">
         <v>2</v>
@@ -31122,7 +31634,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="42" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G3" s="11">
         <f t="shared" ref="G3:G36" si="0">SUM(H3:AL3)</f>
@@ -31182,7 +31694,7 @@
     <row r="4" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="116">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="117">
         <v>2</v>
@@ -31194,7 +31706,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="11">
         <f t="shared" si="0"/>
@@ -31253,20 +31765,20 @@
     </row>
     <row r="5" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="156">
+      <c r="B5" s="154">
         <v>84</v>
       </c>
-      <c r="C5" s="157">
+      <c r="C5" s="155">
         <v>2</v>
       </c>
-      <c r="D5" s="157">
+      <c r="D5" s="155">
         <v>42</v>
       </c>
-      <c r="E5" s="159">
+      <c r="E5" s="157">
         <v>0</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="11">
         <f t="shared" si="0"/>
@@ -33695,12 +34207,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33773,8 +34285,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="154"/>
-      <c r="AR1" s="155"/>
+      <c r="AQ1" s="159"/>
+      <c r="AR1" s="160"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -36426,12 +36938,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36504,8 +37016,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -39204,12 +39716,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39281,8 +39793,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="154"/>
-      <c r="AS1" s="155"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -41981,12 +42493,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42057,8 +42569,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="154"/>
-      <c r="AR1" s="155"/>
+      <c r="AQ1" s="159"/>
+      <c r="AR1" s="160"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -44710,12 +45222,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Esfuerzos y los problemas y lecciones aprendidas
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Iñigo.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Iñigo.xlsx
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="57">
   <si>
     <t>GP</t>
   </si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>Auditoría terminar</t>
+  </si>
+  <si>
+    <t>Documentación</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1882,63 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2464,7 +2523,7 @@
                   <c:v>7.55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2561,11 +2620,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="304041120"/>
-        <c:axId val="231855392"/>
+        <c:axId val="301006136"/>
+        <c:axId val="226414008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="304041120"/>
+        <c:axId val="301006136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2606,7 +2665,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231855392"/>
+        <c:crossAx val="226414008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2614,7 +2673,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231855392"/>
+        <c:axId val="226414008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2670,7 +2729,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304041120"/>
+        <c:crossAx val="301006136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3434,6 +3493,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10610850" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4234,6 +4341,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5002,6 +5157,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5738,6 +5941,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6563,6 +6814,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7299,6 +7598,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8099,6 +8446,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8835,6 +9230,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -9635,6 +10078,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10371,6 +10862,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -11171,6 +11710,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11939,6 +12526,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14877,10 +15512,10 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17709,12 +18344,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20494,12 +21129,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23328,12 +23963,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23556,7 +24191,7 @@
       </c>
       <c r="G6" s="82">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>34.049999999999997</v>
+        <v>41.05</v>
       </c>
       <c r="H6" s="84">
         <f>Ene!G36</f>
@@ -23576,7 +24211,7 @@
       </c>
       <c r="L6" s="84">
         <f>May!G36</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M6" s="84">
         <f>Jun!G36</f>
@@ -24113,12 +24748,12 @@
     <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26804,30 +27439,30 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G35">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G35">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5">
-    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29681,30 +30316,30 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G8 G10:G35">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G8 G10:G35">
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3 G9">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3 G9">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29720,7 +30355,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="B11:F11"/>
+      <selection activeCell="F12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32549,22 +33184,22 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G11 G13:G35">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G11 G13:G35">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32580,7 +33215,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -33227,7 +33862,9 @@
       <c r="C9" s="117">
         <v>2</v>
       </c>
-      <c r="D9" s="20"/>
+      <c r="D9" s="20">
+        <v>58</v>
+      </c>
       <c r="E9" s="157">
         <v>0</v>
       </c>
@@ -33363,14 +34000,24 @@
     </row>
     <row r="11" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="154">
+        <v>84</v>
+      </c>
+      <c r="C11" s="117">
+        <v>2</v>
+      </c>
+      <c r="D11" s="20">
+        <v>44</v>
+      </c>
+      <c r="E11" s="157">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="G11" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(H11:AL11)</f>
+        <v>1</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -33382,7 +34029,9 @@
       <c r="O11" s="20"/>
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
-      <c r="R11" s="20"/>
+      <c r="R11" s="20">
+        <v>1</v>
+      </c>
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
       <c r="U11" s="20"/>
@@ -33423,14 +34072,22 @@
     </row>
     <row r="12" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="154">
+        <v>84</v>
+      </c>
+      <c r="C12" s="155">
+        <v>2</v>
+      </c>
+      <c r="D12" s="155">
+        <v>44</v>
+      </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
+      <c r="F12" s="156" t="s">
+        <v>47</v>
+      </c>
       <c r="G12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -33444,7 +34101,9 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
+      <c r="T12" s="20">
+        <v>2</v>
+      </c>
       <c r="U12" s="20"/>
       <c r="V12" s="20"/>
       <c r="W12" s="16"/>
@@ -33483,14 +34142,24 @@
     </row>
     <row r="13" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="B13" s="154">
+        <v>84</v>
+      </c>
+      <c r="C13" s="117">
+        <v>2</v>
+      </c>
+      <c r="D13" s="20">
+        <v>58</v>
+      </c>
+      <c r="E13" s="157">
+        <v>0</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="G13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -33500,7 +34169,9 @@
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
-      <c r="P13" s="16"/>
+      <c r="P13" s="16">
+        <v>2</v>
+      </c>
       <c r="Q13" s="16"/>
       <c r="R13" s="20"/>
       <c r="S13" s="20"/>
@@ -33543,14 +34214,22 @@
     </row>
     <row r="14" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="B14" s="18">
+        <v>84</v>
+      </c>
+      <c r="C14" s="20">
+        <v>2</v>
+      </c>
+      <c r="D14" s="20">
+        <v>57</v>
+      </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
+      <c r="F14" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="G14" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
@@ -33571,7 +34250,9 @@
       <c r="X14" s="16"/>
       <c r="Y14" s="20"/>
       <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
+      <c r="AA14" s="20">
+        <v>1</v>
+      </c>
       <c r="AB14" s="20"/>
       <c r="AC14" s="20"/>
       <c r="AD14" s="16"/>
@@ -33603,14 +34284,22 @@
     </row>
     <row r="15" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="B15" s="18">
+        <v>84</v>
+      </c>
+      <c r="C15" s="20">
+        <v>2</v>
+      </c>
+      <c r="D15" s="20">
+        <v>57</v>
+      </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
+      <c r="F15" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="G15" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="G15" si="1">SUM(H15:AL15)</f>
+        <v>1</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -33633,7 +34322,9 @@
       <c r="Z15" s="20"/>
       <c r="AA15" s="20"/>
       <c r="AB15" s="20"/>
-      <c r="AC15" s="20"/>
+      <c r="AC15" s="20">
+        <v>1</v>
+      </c>
       <c r="AD15" s="16"/>
       <c r="AE15" s="16"/>
       <c r="AF15" s="20"/>
@@ -34872,130 +35563,130 @@
       </c>
       <c r="G36" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H36" s="34">
-        <f t="shared" ref="H36:AL36" si="1">SUM(H3:H35)</f>
+        <f t="shared" ref="H36:AL36" si="2">SUM(H3:H35)</f>
         <v>0</v>
       </c>
       <c r="I36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="P36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q36" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="51">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S36" s="51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="51">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Q36" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R36" s="51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S36" s="51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T36" s="51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="U36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="W36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Y36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA36" s="51">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="AB36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC36" s="51">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="AD36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AL36" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM36" s="1"/>
@@ -35432,13 +36123,23 @@
   <mergeCells count="1">
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="G3:G14 G16:G35">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="G3:G14 G16:G35">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38164,12 +38865,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40942,12 +41643,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43719,12 +44420,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46448,12 +47149,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>